<commit_message>
Neue Zeiterfassung + Neue Einteilung
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
   <si>
     <t>Datum</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>Wordpress vorbereitet (für den Online Blog                   OPV Testschaltung</t>
+  </si>
+  <si>
+    <t>Lastenheft fertiggestellt</t>
+  </si>
+  <si>
+    <t>Einrichtung Access Point</t>
   </si>
 </sst>
 </file>
@@ -1755,8 +1761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2183,12 +2189,22 @@
         <f t="shared" si="1"/>
         <v>42056</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="D27" s="9"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
+      <c r="E27" s="12">
+        <v>2</v>
+      </c>
+      <c r="F27" s="12">
+        <v>2</v>
+      </c>
+      <c r="G27" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="H27" s="12">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
@@ -2215,12 +2231,22 @@
         <f t="shared" si="1"/>
         <v>42058</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="D29" s="9"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
+      <c r="E29" s="12">
+        <v>2</v>
+      </c>
+      <c r="F29" s="12">
+        <v>2</v>
+      </c>
+      <c r="G29" s="12">
+        <v>0</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
@@ -2310,7 +2336,7 @@
       <c r="C35" s="34"/>
       <c r="D35" s="20">
         <f>SUM(E4:H34)</f>
-        <v>17</v>
+        <v>25.6</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>

</xml_diff>

<commit_message>
Update Zeiterfassung + Projekthandbuch
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="228" windowWidth="18540" windowHeight="8892" tabRatio="882" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="228" windowWidth="18540" windowHeight="8892" tabRatio="882" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Januar" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
   <si>
     <t>Datum</t>
   </si>
@@ -68,15 +68,6 @@
   </si>
   <si>
     <t>Testen abgeschlossen</t>
-  </si>
-  <si>
-    <t>Vorbereitung des Plüschtiers abgeschlossen</t>
-  </si>
-  <si>
-    <t>Einbau und Verkabeln der Komponenten abgeschlossen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finales Testen (inkl. Fehlerbehebung) des kompletten Plüschtiers </t>
   </si>
   <si>
     <t>Projektabschlussbericht übergeben</t>
@@ -138,6 +129,63 @@
   </si>
   <si>
     <t>DHCP, Android App, Testen</t>
+  </si>
+  <si>
+    <t>App Development - Sensoren Code</t>
+  </si>
+  <si>
+    <t>Produktbeschreibung + Logo</t>
+  </si>
+  <si>
+    <t>Ferien</t>
+  </si>
+  <si>
+    <t>Budapest</t>
+  </si>
+  <si>
+    <t>[Vorbereitung des Plüschtiers abgeschlossen] Budapest</t>
+  </si>
+  <si>
+    <t>Medientechnik - Filmtechnik</t>
+  </si>
+  <si>
+    <t>Erweiterte Tests und Planung</t>
+  </si>
+  <si>
+    <t>Sivan,Pavic</t>
+  </si>
+  <si>
+    <t>Webblog + Software</t>
+  </si>
+  <si>
+    <t>[Einbau und Verkabeln der Komponenten abgeschlossen]</t>
+  </si>
+  <si>
+    <t>Planung - Software</t>
+  </si>
+  <si>
+    <t>Logo neu</t>
+  </si>
+  <si>
+    <t>Planung - Software, App</t>
+  </si>
+  <si>
+    <t>Planung - Software,App</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taster anlöten </t>
+  </si>
+  <si>
+    <t>Frei</t>
+  </si>
+  <si>
+    <t>Planung - Software, App, Hardware vollständig</t>
+  </si>
+  <si>
+    <t>[Finales Testen (inkl. Fehlerbehebung) des kompletten Plüschtiers ], Planung - Software</t>
+  </si>
+  <si>
+    <t>Projekthandbuch start</t>
   </si>
 </sst>
 </file>
@@ -429,6 +477,9 @@
     <xf numFmtId="167" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -455,9 +506,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1141,7 +1189,7 @@
   <dimension ref="A2:K49"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1155,29 +1203,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="32">
+      <c r="A3" s="33">
         <f>A7</f>
         <v>42005</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -1692,8 +1740,12 @@
       <c r="F35" s="12">
         <v>0.1</v>
       </c>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
+      <c r="G35" s="12">
+        <v>0</v>
+      </c>
+      <c r="H35" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
@@ -1728,11 +1780,11 @@
       <c r="H37" s="26"/>
     </row>
     <row r="38" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
+      <c r="A38" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="35"/>
+      <c r="C38" s="36"/>
       <c r="D38" s="20">
         <f>SUM(E7:H37)</f>
         <v>2.6</v>
@@ -1821,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1834,29 +1886,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="38">
+      <c r="A3" s="39">
         <f>A7</f>
         <v>42036</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -2026,7 +2078,7 @@
         <v>42044</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="17"/>
@@ -2044,7 +2096,7 @@
         <v>42045</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="12">
@@ -2070,7 +2122,7 @@
         <v>42046</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="12">
@@ -2160,7 +2212,7 @@
         <v>42051</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="17">
@@ -2250,7 +2302,7 @@
         <v>42056</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="12">
@@ -2292,7 +2344,7 @@
         <v>42058</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="12">
@@ -2318,7 +2370,7 @@
         <v>42059</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="12">
@@ -2344,17 +2396,21 @@
         <v>42060</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="12">
         <v>2.5</v>
       </c>
-      <c r="F31" s="12"/>
+      <c r="F31" s="12">
+        <v>0</v>
+      </c>
       <c r="G31" s="12">
         <v>0.5</v>
       </c>
-      <c r="H31" s="12"/>
+      <c r="H31" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
@@ -2405,28 +2461,28 @@
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="35"/>
+      <c r="A35" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="35"/>
+      <c r="C35" s="36"/>
       <c r="D35" s="20">
         <f>SUM(E4:H34)</f>
         <v>37.6</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="30">
         <f>SUM(E7:E34)</f>
         <v>14.9</v>
       </c>
-      <c r="F35" s="39">
+      <c r="F35" s="30">
         <f>SUM(F7:F34)</f>
         <v>11.1</v>
       </c>
-      <c r="G35" s="39">
+      <c r="G35" s="30">
         <f>SUM(G7:G34)</f>
         <v>4.8999999999999995</v>
       </c>
-      <c r="H35" s="39">
+      <c r="H35" s="30">
         <f>SUM(H7:H34)</f>
         <v>6.7</v>
       </c>
@@ -2489,8 +2545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:H38"/>
+    <sheetView topLeftCell="A19" zoomScale="94" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2503,29 +2559,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="32">
+      <c r="A3" s="33">
         <f>A7</f>
         <v>42064</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -2567,7 +2623,7 @@
         <v>42064</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10">
@@ -2609,7 +2665,7 @@
         <v>42066</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="12">
@@ -2715,7 +2771,7 @@
         <v>42072</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="17">
@@ -2741,7 +2797,7 @@
         <v>42073</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="12">
@@ -2847,7 +2903,7 @@
         <v>42079</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>8</v>
@@ -2875,10 +2931,10 @@
         <v>42080</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E23" s="12">
         <v>5</v>
@@ -2903,7 +2959,7 @@
         <v>42081</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>9</v>
@@ -2996,12 +3052,22 @@
         <f t="shared" si="1"/>
         <v>42086</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="D29" s="9"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
+      <c r="E29" s="12">
+        <v>2</v>
+      </c>
+      <c r="F29" s="12">
+        <v>2</v>
+      </c>
+      <c r="G29" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
@@ -3028,12 +3094,22 @@
         <f t="shared" si="1"/>
         <v>42088</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="D31" s="9"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="E31" s="12">
+        <v>2</v>
+      </c>
+      <c r="F31" s="12">
+        <v>1</v>
+      </c>
+      <c r="G31" s="12">
+        <v>2</v>
+      </c>
+      <c r="H31" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
@@ -3076,7 +3152,9 @@
         <f t="shared" si="1"/>
         <v>42091</v>
       </c>
-      <c r="C34" s="11"/>
+      <c r="C34" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="D34" s="9"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
@@ -3108,14 +3186,16 @@
         <f t="shared" si="1"/>
         <v>42093</v>
       </c>
-      <c r="C36" s="11"/>
+      <c r="C36" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="D36" s="9"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
     </row>
-    <row r="37" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="13">
         <f t="shared" si="0"/>
         <v>42094</v>
@@ -3125,7 +3205,7 @@
         <v>42094</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="27"/>
@@ -3134,30 +3214,30 @@
       <c r="H37" s="27"/>
     </row>
     <row r="38" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
+      <c r="A38" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="35"/>
+      <c r="C38" s="36"/>
       <c r="D38" s="20">
         <f>SUM(E7:H37)</f>
-        <v>45.5</v>
-      </c>
-      <c r="E38" s="39">
+        <v>57.5</v>
+      </c>
+      <c r="E38" s="30">
         <f>SUM(E7:E37)</f>
-        <v>18.5</v>
-      </c>
-      <c r="F38" s="39">
+        <v>22.5</v>
+      </c>
+      <c r="F38" s="30">
         <f>SUM(F7:F37)</f>
-        <v>19</v>
-      </c>
-      <c r="G38" s="39">
+        <v>22</v>
+      </c>
+      <c r="G38" s="30">
         <f>SUM(G7:G37)</f>
-        <v>5</v>
-      </c>
-      <c r="H38" s="39">
+        <v>7.5</v>
+      </c>
+      <c r="H38" s="30">
         <f>SUM(H7:H37)</f>
-        <v>3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3213,8 +3293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3227,29 +3307,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="32">
+      <c r="A3" s="33">
         <f>A7</f>
         <v>42095</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -3290,7 +3370,9 @@
         <f>A7</f>
         <v>42095</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -3306,12 +3388,24 @@
         <f>B7+1</f>
         <v>42096</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="C8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="10">
+        <v>2</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2</v>
+      </c>
+      <c r="G8" s="10">
+        <v>2</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
@@ -3361,7 +3455,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>42100</v>
@@ -3370,12 +3464,24 @@
         <f t="shared" si="1"/>
         <v>42100</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="C12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="12">
+        <v>2</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
@@ -3402,12 +3508,22 @@
         <f t="shared" si="1"/>
         <v>42102</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="D14" s="9"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="E14" s="12">
+        <v>1</v>
+      </c>
+      <c r="F14" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
@@ -3482,12 +3598,22 @@
         <f t="shared" si="1"/>
         <v>42107</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
+      <c r="E19" s="12">
+        <v>2</v>
+      </c>
+      <c r="F19" s="12">
+        <v>2</v>
+      </c>
+      <c r="G19" s="12">
+        <v>2</v>
+      </c>
+      <c r="H19" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
@@ -3498,12 +3624,22 @@
         <f t="shared" si="1"/>
         <v>42108</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D20" s="9"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
+      <c r="E20" s="12">
+        <v>0</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
@@ -3515,7 +3651,7 @@
         <v>42109</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="17"/>
@@ -3596,12 +3732,24 @@
         <f t="shared" si="1"/>
         <v>42114</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
+      <c r="C26" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="12">
+        <v>2</v>
+      </c>
+      <c r="F26" s="12">
+        <v>2</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -3628,12 +3776,22 @@
         <f t="shared" si="1"/>
         <v>42116</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="D28" s="9"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
+      <c r="E28" s="12">
+        <v>2</v>
+      </c>
+      <c r="F28" s="12">
+        <v>2</v>
+      </c>
+      <c r="G28" s="12">
+        <v>1</v>
+      </c>
+      <c r="H28" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
@@ -3708,12 +3866,22 @@
         <f t="shared" si="1"/>
         <v>42121</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C33" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="D33" s="9"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
+      <c r="E33" s="12">
+        <v>2</v>
+      </c>
+      <c r="F33" s="12">
+        <v>2</v>
+      </c>
+      <c r="G33" s="12">
+        <v>2</v>
+      </c>
+      <c r="H33" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
@@ -3724,12 +3892,24 @@
         <f t="shared" si="1"/>
         <v>42122</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
+      <c r="C34" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0</v>
+      </c>
+      <c r="F34" s="12">
+        <v>2</v>
+      </c>
+      <c r="G34" s="12">
+        <v>2</v>
+      </c>
+      <c r="H34" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
@@ -3740,12 +3920,22 @@
         <f t="shared" si="1"/>
         <v>42123</v>
       </c>
-      <c r="C35" s="11"/>
+      <c r="C35" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="D35" s="9"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
+      <c r="E35" s="12">
+        <v>2</v>
+      </c>
+      <c r="F35" s="12">
+        <v>2</v>
+      </c>
+      <c r="G35" s="12">
+        <v>2</v>
+      </c>
+      <c r="H35" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
@@ -3764,30 +3954,30 @@
       <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="35"/>
+      <c r="A37" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="35"/>
+      <c r="C37" s="36"/>
       <c r="D37" s="20">
         <f>SUM(E6:H36)</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="39">
+        <v>56</v>
+      </c>
+      <c r="E37" s="30">
         <f>SUM(E7:E36)</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="39">
+        <v>15</v>
+      </c>
+      <c r="F37" s="30">
         <f>SUM(F7:F36)</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="39">
+        <v>17.5</v>
+      </c>
+      <c r="G37" s="30">
         <f>SUM(G7:G36)</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="39">
+        <v>13.5</v>
+      </c>
+      <c r="H37" s="30">
         <f>SUM(H7:H36)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3835,8 +4025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3848,29 +4038,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="38">
+      <c r="A3" s="39">
         <f>A7</f>
         <v>42125</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -3911,7 +4101,9 @@
         <f>A7</f>
         <v>42125</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -3959,12 +4151,24 @@
         <f t="shared" si="1"/>
         <v>42128</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="C10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="12">
+        <v>2</v>
+      </c>
+      <c r="F10" s="12">
+        <v>2</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -3982,7 +4186,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>42130</v>
@@ -3991,12 +4195,24 @@
         <f t="shared" si="1"/>
         <v>42130</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="C12" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="12">
+        <v>2</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
@@ -4072,13 +4288,21 @@
         <v>42135</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="E17" s="17">
+        <v>2</v>
+      </c>
+      <c r="F17" s="17">
+        <v>2</v>
+      </c>
+      <c r="G17" s="17">
+        <v>2</v>
+      </c>
+      <c r="H17" s="17">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
@@ -4089,12 +4313,22 @@
         <f t="shared" si="1"/>
         <v>42136</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
+      <c r="E18" s="12">
+        <v>2</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12">
+        <v>0</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
@@ -4298,7 +4532,7 @@
         <v>42149</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="17"/>
@@ -4403,14 +4637,14 @@
       <c r="H37" s="26"/>
     </row>
     <row r="38" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
+      <c r="A38" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="35"/>
+      <c r="C38" s="36"/>
       <c r="D38" s="20">
         <f>SUM(E7:H37)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>

</xml_diff>